<commit_message>
Update Excel-template / pivot
It now shows the packages and their licenses. Anyways, assumption is
that whomever wants to use this this tool gets along with Excel or
their other spreadsheet program well enough.
</commit_message>
<xml_diff>
--- a/excel-template.xlsx
+++ b/excel-template.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\licensetool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanneKiiskilä\git\licensetool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BDA8DB-A612-404F-B6F6-51A6F4459375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F64D5F3-EAA7-488F-9048-3DE7E606DFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Analysis" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="15" r:id="rId2"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,6 +34,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Count of Package</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>GPLv2+</t>
+  </si>
+  <si>
+    <t>MPL-2.0</t>
+  </si>
+  <si>
+    <t>MPL-2.0-changed</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64,8 +99,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -81,6 +121,274 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Janne Kiiskilä" refreshedDate="44512.668733217593" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="7" xr:uid="{9B89DEC9-2841-403D-BE05-BF2F73C7954A}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:L1048576" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="12">
+    <cacheField name="Package" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Previous version" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Previous recipe" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Previous license" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Current version" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Current recipe" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Current license" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="GPLv2+"/>
+        <m/>
+        <s v="MPL-2.0-changed"/>
+        <s v="MPL-2.0"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Change" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="y"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Version change" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="y"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="License change" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Package added" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <m/>
+        <s v="y"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Package removed" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <m/>
+        <s v="y"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="7">
+  <r>
+    <s v="acl"/>
+    <s v="2.2.53"/>
+    <s v="acl"/>
+    <s v="GPLv2+"/>
+    <s v="3.2.53"/>
+    <s v="acl"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="acl-dev"/>
+    <s v="2.2.53"/>
+    <s v="acl"/>
+    <s v="LGPLv2.1+ &amp; GPLv2+"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="aktualizr-configs"/>
+    <s v="1.0+gitAUTOINC+dad22588d7"/>
+    <s v="aktualizr"/>
+    <s v="MPL-2.0"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="aktualizr"/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="1.0+gitAUTOINC+dad22588d7"/>
+    <s v="aktualizr"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="New-Package"/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="1.0"/>
+    <s v="New-Package"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7EC6FF04-7C7E-470B-975D-6636E22E51B3}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="12">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="7" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Package" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,18 +654,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <f>1+1</f>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>